<commit_message>
Final update with multiple changes
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hydroweb\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hydroweb\IdeaProjects\DemoExerciseJodaynTest\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEEBCEA4-42F5-47E6-B5CC-EFB9B81FB4F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE1F6D84-471E-4F41-833E-FB3DEDDA4219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4815" yWindow="2655" windowWidth="15375" windowHeight="7875" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11295" yWindow="2025" windowWidth="9525" windowHeight="7875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ExistingUser" sheetId="1" r:id="rId1"/>
@@ -151,9 +151,6 @@
     <t>Irqah 7020</t>
   </si>
   <si>
-    <t>585150202</t>
-  </si>
-  <si>
     <t>Bilal Imam</t>
   </si>
   <si>
@@ -169,9 +166,6 @@
     <t>Test@1994</t>
   </si>
   <si>
-    <t>Dashboard</t>
-  </si>
-  <si>
     <t>New Orleans</t>
   </si>
   <si>
@@ -179,6 +173,12 @@
   </si>
   <si>
     <t>12345</t>
+  </si>
+  <si>
+    <t>Karachi 2020</t>
+  </si>
+  <si>
+    <t>536691048</t>
   </si>
 </sst>
 </file>
@@ -579,13 +579,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -604,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,8 +618,9 @@
     <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" customWidth="1"/>
     <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -688,22 +689,22 @@
         <v>39</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>12</v>
       </c>
       <c r="J2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="L2" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="K2" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>49</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -771,7 +772,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49FEA492-6320-4DEE-8D23-6B2D7C33D1BC}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -803,7 +804,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" s="4">
         <v>548951612311321</v>
@@ -812,7 +813,7 @@
         <v>194</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E2">
         <v>2027</v>

</xml_diff>